<commit_message>
committing AP Call Update
AP Voice Mail List
</commit_message>
<xml_diff>
--- a/campaign/Advance Poll Kit/AdvancePoll.call-list.xlsx
+++ b/campaign/Advance Poll Kit/AdvancePoll.call-list.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2887" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="782">
   <si>
     <t>VotedOn</t>
   </si>
@@ -2357,6 +2357,12 @@
   </si>
   <si>
     <t>Talk to in Person</t>
+  </si>
+  <si>
+    <t>NO VM</t>
+  </si>
+  <si>
+    <t>Voted and Supported us</t>
   </si>
 </sst>
 </file>
@@ -2795,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M423"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
+      <selection activeCell="M305" sqref="M305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2806,7 +2812,7 @@
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -11504,7 +11510,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="241" spans="1:12">
+    <row r="241" spans="1:13">
       <c r="A241" s="2"/>
       <c r="B241">
         <v>5</v>
@@ -11537,7 +11543,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="242" spans="1:12">
+    <row r="242" spans="1:13">
       <c r="A242" s="2"/>
       <c r="B242">
         <v>5</v>
@@ -11570,7 +11576,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="243" spans="1:12">
+    <row r="243" spans="1:13">
       <c r="A243" s="2"/>
       <c r="B243">
         <v>5</v>
@@ -11606,7 +11612,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="244" spans="1:12">
+    <row r="244" spans="1:13">
       <c r="A244" s="2"/>
       <c r="B244">
         <v>5</v>
@@ -11642,7 +11648,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="245" spans="1:12">
+    <row r="245" spans="1:13">
       <c r="A245" s="2"/>
       <c r="B245">
         <v>5</v>
@@ -11678,7 +11684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:12">
+    <row r="246" spans="1:13">
       <c r="A246" s="2"/>
       <c r="B246">
         <v>5</v>
@@ -11714,7 +11720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="1:12">
+    <row r="247" spans="1:13">
       <c r="A247" s="2"/>
       <c r="B247">
         <v>5</v>
@@ -11750,7 +11756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="248" spans="1:12">
+    <row r="248" spans="1:13">
       <c r="A248" s="2"/>
       <c r="B248">
         <v>5</v>
@@ -11786,7 +11792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="249" spans="1:12">
+    <row r="249" spans="1:13">
       <c r="A249" s="2"/>
       <c r="B249">
         <v>5</v>
@@ -11822,7 +11828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="250" spans="1:12">
+    <row r="250" spans="1:13">
       <c r="A250" s="2"/>
       <c r="B250">
         <v>5</v>
@@ -11858,7 +11864,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="251" spans="1:12">
+    <row r="251" spans="1:13">
       <c r="A251" s="2"/>
       <c r="B251">
         <v>5</v>
@@ -11894,7 +11900,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="252" spans="1:12">
+    <row r="252" spans="1:13">
       <c r="A252" s="2"/>
       <c r="B252">
         <v>5</v>
@@ -11927,7 +11933,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="253" spans="1:12">
+    <row r="253" spans="1:13">
       <c r="A253" s="2"/>
       <c r="B253">
         <v>5</v>
@@ -11963,7 +11969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="254" spans="1:12">
+    <row r="254" spans="1:13">
       <c r="A254" s="2"/>
       <c r="B254">
         <v>5</v>
@@ -11999,7 +12005,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="255" spans="1:12">
+    <row r="255" spans="1:13">
       <c r="A255" s="2"/>
       <c r="B255">
         <v>5</v>
@@ -12034,8 +12040,11 @@
       <c r="L255" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="256" spans="1:12">
+      <c r="M255" s="2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13">
       <c r="A256" s="2"/>
       <c r="B256">
         <v>5</v>
@@ -12070,8 +12079,11 @@
       <c r="L256" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="257" spans="1:12">
+      <c r="M256" s="2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13">
       <c r="A257" s="2"/>
       <c r="B257">
         <v>5</v>
@@ -12107,7 +12119,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="258" spans="1:12">
+    <row r="258" spans="1:13">
       <c r="A258" s="2"/>
       <c r="B258">
         <v>5</v>
@@ -12143,7 +12155,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="259" spans="1:12">
+    <row r="259" spans="1:13">
       <c r="A259" s="2"/>
       <c r="B259">
         <v>5</v>
@@ -12179,7 +12191,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="260" spans="1:12">
+    <row r="260" spans="1:13">
       <c r="A260" s="2"/>
       <c r="B260">
         <v>5</v>
@@ -12215,7 +12227,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="261" spans="1:12">
+    <row r="261" spans="1:13">
       <c r="A261" s="2"/>
       <c r="B261">
         <v>5</v>
@@ -12251,7 +12263,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="262" spans="1:12">
+    <row r="262" spans="1:13">
       <c r="A262" s="2"/>
       <c r="B262">
         <v>5</v>
@@ -12287,7 +12299,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="263" spans="1:12">
+    <row r="263" spans="1:13">
       <c r="A263" s="2"/>
       <c r="B263">
         <v>5</v>
@@ -12323,7 +12335,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="264" spans="1:12">
+    <row r="264" spans="1:13">
       <c r="A264" s="2"/>
       <c r="B264">
         <v>5</v>
@@ -12359,7 +12371,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="265" spans="1:12">
+    <row r="265" spans="1:13">
       <c r="A265" s="2"/>
       <c r="B265">
         <v>5</v>
@@ -12394,8 +12406,11 @@
       <c r="L265" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="266" spans="1:12">
+      <c r="M265" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13">
       <c r="A266" s="2"/>
       <c r="B266">
         <v>5</v>
@@ -12430,8 +12445,11 @@
       <c r="L266" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="267" spans="1:12">
+      <c r="M266" s="2" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13">
       <c r="A267" s="2"/>
       <c r="B267">
         <v>5</v>
@@ -12463,8 +12481,11 @@
       <c r="L267" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="268" spans="1:12">
+      <c r="M267" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13">
       <c r="A268" s="2"/>
       <c r="B268">
         <v>5</v>
@@ -12496,8 +12517,11 @@
       <c r="L268" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="269" spans="1:12">
+      <c r="M268" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13">
       <c r="A269" s="2"/>
       <c r="B269">
         <v>5</v>
@@ -12529,8 +12553,11 @@
       <c r="L269" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="270" spans="1:12">
+      <c r="M269" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13">
       <c r="A270" s="2"/>
       <c r="B270">
         <v>5</v>
@@ -12562,8 +12589,11 @@
       <c r="L270" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="271" spans="1:12">
+      <c r="M270" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13">
       <c r="A271" s="2"/>
       <c r="B271">
         <v>5</v>
@@ -12596,7 +12626,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="272" spans="1:12">
+    <row r="272" spans="1:13">
       <c r="A272" s="2"/>
       <c r="B272">
         <v>5</v>
@@ -12628,8 +12658,11 @@
       <c r="L272" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="273" spans="1:12">
+      <c r="M272" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13">
       <c r="A273" s="2"/>
       <c r="B273">
         <v>5</v>
@@ -12661,8 +12694,11 @@
       <c r="L273" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="274" spans="1:12">
+      <c r="M273" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13">
       <c r="A274" s="2"/>
       <c r="B274">
         <v>5</v>
@@ -12695,7 +12731,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="1:12">
+    <row r="275" spans="1:13">
       <c r="A275" s="2"/>
       <c r="B275">
         <v>5</v>
@@ -12728,7 +12764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="276" spans="1:12">
+    <row r="276" spans="1:13">
       <c r="A276" s="2"/>
       <c r="B276">
         <v>5</v>
@@ -12760,8 +12796,11 @@
       <c r="L276" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="277" spans="1:12">
+      <c r="M276" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13">
       <c r="A277" s="2"/>
       <c r="B277">
         <v>5</v>
@@ -12793,8 +12832,11 @@
       <c r="L277" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="278" spans="1:12">
+      <c r="M277" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13">
       <c r="A278" s="2"/>
       <c r="B278">
         <v>5</v>
@@ -12827,7 +12869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="279" spans="1:12">
+    <row r="279" spans="1:13">
       <c r="A279" s="2"/>
       <c r="B279">
         <v>5</v>
@@ -12860,7 +12902,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="280" spans="1:12">
+    <row r="280" spans="1:13">
       <c r="A280" s="2"/>
       <c r="B280">
         <v>5</v>
@@ -12893,7 +12935,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="281" spans="1:12">
+    <row r="281" spans="1:13">
       <c r="A281" s="2"/>
       <c r="B281">
         <v>5</v>
@@ -12926,7 +12968,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="282" spans="1:12">
+    <row r="282" spans="1:13">
       <c r="A282" s="2"/>
       <c r="B282">
         <v>5</v>
@@ -12959,7 +13001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="283" spans="1:12">
+    <row r="283" spans="1:13">
       <c r="A283" s="2"/>
       <c r="B283">
         <v>5</v>
@@ -12992,7 +13034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="284" spans="1:12">
+    <row r="284" spans="1:13">
       <c r="A284" s="2"/>
       <c r="B284">
         <v>5</v>
@@ -13024,8 +13066,11 @@
       <c r="L284" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="285" spans="1:12">
+      <c r="M284" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13">
       <c r="A285" s="2"/>
       <c r="B285">
         <v>5</v>
@@ -13057,8 +13102,11 @@
       <c r="L285" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="286" spans="1:12">
+      <c r="M285" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13">
       <c r="A286" s="2"/>
       <c r="B286">
         <v>5</v>
@@ -13090,8 +13138,11 @@
       <c r="L286" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="287" spans="1:12">
+      <c r="M286" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13">
       <c r="A287" s="2"/>
       <c r="B287">
         <v>5</v>
@@ -13124,8 +13175,11 @@
       <c r="L287" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="288" spans="1:12">
+      <c r="M287" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13">
       <c r="A288" s="2"/>
       <c r="B288">
         <v>5</v>
@@ -13158,8 +13212,11 @@
       <c r="L288" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="289" spans="1:12">
+      <c r="M288" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13">
       <c r="A289" s="2"/>
       <c r="B289">
         <v>5</v>
@@ -13192,8 +13249,11 @@
       <c r="L289" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="290" spans="1:12">
+      <c r="M289" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13">
       <c r="A290" s="2"/>
       <c r="B290">
         <v>5</v>
@@ -13225,8 +13285,11 @@
       <c r="L290" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="291" spans="1:12">
+      <c r="M290" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13">
       <c r="A291" s="2"/>
       <c r="B291">
         <v>5</v>
@@ -13259,8 +13322,11 @@
       <c r="L291" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="292" spans="1:12">
+      <c r="M291" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13">
       <c r="A292" s="2"/>
       <c r="B292">
         <v>5</v>
@@ -13293,8 +13359,11 @@
       <c r="L292" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="293" spans="1:12">
+      <c r="M292" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="293" spans="1:13">
       <c r="A293" s="2"/>
       <c r="B293">
         <v>5</v>
@@ -13327,8 +13396,11 @@
       <c r="L293" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="294" spans="1:12">
+      <c r="M293" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="294" spans="1:13">
       <c r="A294" s="2"/>
       <c r="B294">
         <v>5</v>
@@ -13361,8 +13433,11 @@
       <c r="L294" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="295" spans="1:12">
+      <c r="M294" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13">
       <c r="A295" s="2"/>
       <c r="B295">
         <v>5</v>
@@ -13395,8 +13470,11 @@
       <c r="L295" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="296" spans="1:12">
+      <c r="M295" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13">
       <c r="A296" s="2"/>
       <c r="B296">
         <v>5</v>
@@ -13430,7 +13508,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="297" spans="1:12">
+    <row r="297" spans="1:13">
       <c r="A297" s="2"/>
       <c r="B297">
         <v>5</v>
@@ -13464,7 +13542,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:12">
+    <row r="298" spans="1:13">
       <c r="A298" s="2"/>
       <c r="B298">
         <v>5</v>
@@ -13498,7 +13576,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="299" spans="1:12">
+    <row r="299" spans="1:13">
       <c r="A299" s="2"/>
       <c r="B299">
         <v>5</v>
@@ -13530,8 +13608,11 @@
       <c r="L299" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="300" spans="1:12">
+      <c r="M299" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13">
       <c r="A300" s="2"/>
       <c r="B300">
         <v>5</v>
@@ -13563,8 +13644,11 @@
       <c r="L300" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="301" spans="1:12">
+      <c r="M300" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13">
       <c r="A301" s="2"/>
       <c r="B301">
         <v>5</v>
@@ -13596,8 +13680,11 @@
       <c r="L301" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="302" spans="1:12">
+      <c r="M301" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13">
       <c r="A302" s="2"/>
       <c r="B302">
         <v>5</v>
@@ -13632,8 +13719,11 @@
       <c r="L302" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="303" spans="1:12">
+      <c r="M302" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13">
       <c r="A303" s="2"/>
       <c r="B303">
         <v>5</v>
@@ -13668,8 +13758,11 @@
       <c r="L303" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="304" spans="1:12">
+      <c r="M303" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13">
       <c r="A304" s="2"/>
       <c r="B304">
         <v>5</v>
@@ -13704,8 +13797,11 @@
       <c r="L304" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="305" spans="1:12">
+      <c r="M304" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13">
       <c r="A305" s="2"/>
       <c r="B305">
         <v>5</v>
@@ -13740,8 +13836,11 @@
       <c r="L305" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="306" spans="1:12">
+      <c r="M305" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13">
       <c r="A306" s="2"/>
       <c r="B306">
         <v>5</v>
@@ -13775,7 +13874,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="307" spans="1:12">
+    <row r="307" spans="1:13">
       <c r="A307" s="2"/>
       <c r="B307">
         <v>5</v>
@@ -13809,7 +13908,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="308" spans="1:12">
+    <row r="308" spans="1:13">
       <c r="A308" s="2"/>
       <c r="B308">
         <v>5</v>
@@ -13843,7 +13942,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="309" spans="1:12">
+    <row r="309" spans="1:13">
       <c r="A309" s="2"/>
       <c r="B309">
         <v>5</v>
@@ -13876,7 +13975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="310" spans="1:12">
+    <row r="310" spans="1:13">
       <c r="A310" s="2"/>
       <c r="B310">
         <v>5</v>
@@ -13909,7 +14008,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="311" spans="1:12">
+    <row r="311" spans="1:13">
       <c r="A311" s="2"/>
       <c r="B311">
         <v>5</v>
@@ -13942,7 +14041,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="312" spans="1:12">
+    <row r="312" spans="1:13">
       <c r="A312" s="2"/>
       <c r="B312">
         <v>5</v>
@@ -13975,7 +14074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="313" spans="1:12">
+    <row r="313" spans="1:13">
       <c r="A313" s="2"/>
       <c r="B313">
         <v>5</v>
@@ -14009,7 +14108,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="314" spans="1:12">
+    <row r="314" spans="1:13">
       <c r="A314" s="2"/>
       <c r="B314">
         <v>5</v>
@@ -14043,7 +14142,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="315" spans="1:12">
+    <row r="315" spans="1:13">
       <c r="A315" s="2"/>
       <c r="B315">
         <v>5</v>
@@ -14077,7 +14176,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="316" spans="1:12">
+    <row r="316" spans="1:13">
       <c r="A316" s="2"/>
       <c r="B316">
         <v>5</v>
@@ -14113,7 +14212,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="317" spans="1:12">
+    <row r="317" spans="1:13">
       <c r="A317" s="2"/>
       <c r="B317">
         <v>5</v>
@@ -14149,7 +14248,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="318" spans="1:12">
+    <row r="318" spans="1:13">
       <c r="A318" s="2"/>
       <c r="B318">
         <v>5</v>
@@ -14185,7 +14284,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="319" spans="1:12">
+    <row r="319" spans="1:13">
       <c r="A319" s="2"/>
       <c r="B319">
         <v>5</v>
@@ -14221,7 +14320,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="320" spans="1:12">
+    <row r="320" spans="1:13">
       <c r="A320" s="2"/>
       <c r="B320">
         <v>5</v>

</xml_diff>